<commit_message>
Modifiche al contenuto di report-checklist.xlsx
Apportate modifiche al file report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.0/report-checklist.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="489">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -639,7 +639,10 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b40e844989^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>MODIFICA DELLA PROGRAMMAZIONE</t>
+    <t>ATTENZIONE SPECIFICA ESAME NON CORRETTA</t>
+  </si>
+  <si>
+    <t>CORREZIONE DEI DATI ERRATI</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -658,6 +661,9 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.f68c9c6a69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
+    <t>ATTENZIONE MANCA LA SPECIFICA DEL TIPO DI CAMPIONE</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT16_KO</t>
   </si>
   <si>
@@ -672,6 +678,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.683ad8df8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ATTENZIONE MANCA LA SPECIFICA DEL CODICE DELL'ESAME ISOLATO</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -1841,11 +1850,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1941,6 +1950,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1948,8 +1965,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1963,6 +2011,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1972,7 +2043,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1988,90 +2081,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2118,7 +2127,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2130,7 +2157,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2142,13 +2169,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2160,25 +2187,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2190,7 +2199,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2208,49 +2223,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2268,37 +2283,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2622,6 +2631,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2647,47 +2680,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -2704,6 +2696,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -2711,11 +2714,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2723,142 +2732,142 @@
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4500,11 +4509,11 @@
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="N10" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:D5"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4533333333333" defaultRowHeight="15" customHeight="1"/>
@@ -6170,20 +6179,22 @@
         <v>54</v>
       </c>
       <c r="N41" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="O41" s="37"/>
+        <v>54</v>
+      </c>
+      <c r="O41" s="37" t="s">
+        <v>139</v>
+      </c>
       <c r="P41" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Q41" s="37" t="s">
         <v>58</v>
       </c>
       <c r="R41" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="S41" s="37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="T41" s="37"/>
       <c r="U41" s="44"/>
@@ -6203,22 +6214,22 @@
         <v>48</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E42" s="32" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F42" s="35">
         <v>45786</v>
       </c>
       <c r="G42" s="35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H42" s="35" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I42" s="38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J42" s="37" t="s">
         <v>54</v>
@@ -6229,20 +6240,22 @@
         <v>54</v>
       </c>
       <c r="N42" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="O42" s="37"/>
+        <v>54</v>
+      </c>
+      <c r="O42" s="37" t="s">
+        <v>146</v>
+      </c>
       <c r="P42" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Q42" s="37" t="s">
         <v>58</v>
       </c>
       <c r="R42" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="S42" s="37" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="T42" s="37"/>
       <c r="U42" s="44"/>
@@ -6262,22 +6275,22 @@
         <v>48</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E43" s="32" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F43" s="35">
         <v>45786</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I43" s="38" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J43" s="37" t="s">
         <v>54</v>
@@ -6288,20 +6301,22 @@
         <v>54</v>
       </c>
       <c r="N43" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="O43" s="37"/>
+        <v>54</v>
+      </c>
+      <c r="O43" s="37" t="s">
+        <v>152</v>
+      </c>
       <c r="P43" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Q43" s="37" t="s">
         <v>58</v>
       </c>
       <c r="R43" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="S43" s="37" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="T43" s="37"/>
       <c r="U43" s="44"/>
@@ -6321,10 +6336,10 @@
         <v>61</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E44" s="32" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -6358,10 +6373,10 @@
         <v>61</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
@@ -6395,10 +6410,10 @@
         <v>61</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F46" s="35"/>
       <c r="G46" s="35"/>
@@ -6432,10 +6447,10 @@
         <v>61</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F47" s="35"/>
       <c r="G47" s="35"/>
@@ -6469,10 +6484,10 @@
         <v>61</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F48" s="35"/>
       <c r="G48" s="35"/>
@@ -6506,10 +6521,10 @@
         <v>61</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="35"/>
@@ -6543,10 +6558,10 @@
         <v>61</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="35"/>
@@ -6580,10 +6595,10 @@
         <v>61</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="35"/>
@@ -6617,10 +6632,10 @@
         <v>61</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F52" s="35"/>
       <c r="G52" s="35"/>
@@ -6654,10 +6669,10 @@
         <v>61</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E53" s="32" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F53" s="35"/>
       <c r="G53" s="35"/>
@@ -6691,10 +6706,10 @@
         <v>65</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
@@ -6728,10 +6743,10 @@
         <v>65</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F55" s="35"/>
       <c r="G55" s="35"/>
@@ -6765,10 +6780,10 @@
         <v>65</v>
       </c>
       <c r="D56" s="29" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F56" s="35"/>
       <c r="G56" s="35"/>
@@ -6802,10 +6817,10 @@
         <v>65</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E57" s="32" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F57" s="35"/>
       <c r="G57" s="35"/>
@@ -6839,10 +6854,10 @@
         <v>65</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E58" s="32" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F58" s="35"/>
       <c r="G58" s="35"/>
@@ -6876,10 +6891,10 @@
         <v>65</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E59" s="32" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F59" s="35"/>
       <c r="G59" s="35"/>
@@ -6913,10 +6928,10 @@
         <v>65</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E60" s="32" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F60" s="35"/>
       <c r="G60" s="35"/>
@@ -6950,10 +6965,10 @@
         <v>65</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E61" s="32" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F61" s="35"/>
       <c r="G61" s="35"/>
@@ -6987,10 +7002,10 @@
         <v>65</v>
       </c>
       <c r="D62" s="29" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E62" s="32" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F62" s="35"/>
       <c r="G62" s="35"/>
@@ -7024,10 +7039,10 @@
         <v>65</v>
       </c>
       <c r="D63" s="29" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E63" s="32" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F63" s="35"/>
       <c r="G63" s="35"/>
@@ -7061,10 +7076,10 @@
         <v>65</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E64" s="32" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F64" s="35"/>
       <c r="G64" s="35"/>
@@ -7098,10 +7113,10 @@
         <v>65</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E65" s="32" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F65" s="35"/>
       <c r="G65" s="35"/>
@@ -7135,10 +7150,10 @@
         <v>65</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E66" s="32" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F66" s="35"/>
       <c r="G66" s="35"/>
@@ -7172,10 +7187,10 @@
         <v>65</v>
       </c>
       <c r="D67" s="29" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F67" s="35"/>
       <c r="G67" s="35"/>
@@ -7209,10 +7224,10 @@
         <v>65</v>
       </c>
       <c r="D68" s="29" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E68" s="32" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F68" s="35"/>
       <c r="G68" s="35"/>
@@ -7246,10 +7261,10 @@
         <v>65</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E69" s="32" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F69" s="35"/>
       <c r="G69" s="35"/>
@@ -7283,10 +7298,10 @@
         <v>65</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E70" s="32" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F70" s="35"/>
       <c r="G70" s="35"/>
@@ -7320,10 +7335,10 @@
         <v>69</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E71" s="32" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F71" s="35"/>
       <c r="G71" s="35"/>
@@ -7357,10 +7372,10 @@
         <v>69</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E72" s="32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F72" s="35"/>
       <c r="G72" s="35"/>
@@ -7394,10 +7409,10 @@
         <v>69</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E73" s="32" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F73" s="35"/>
       <c r="G73" s="35"/>
@@ -7431,10 +7446,10 @@
         <v>69</v>
       </c>
       <c r="D74" s="29" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E74" s="32" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F74" s="35"/>
       <c r="G74" s="35"/>
@@ -7468,10 +7483,10 @@
         <v>69</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E75" s="32" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F75" s="35"/>
       <c r="G75" s="35"/>
@@ -7505,10 +7520,10 @@
         <v>69</v>
       </c>
       <c r="D76" s="29" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E76" s="32" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F76" s="35"/>
       <c r="G76" s="35"/>
@@ -7542,10 +7557,10 @@
         <v>69</v>
       </c>
       <c r="D77" s="29" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E77" s="32" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F77" s="35"/>
       <c r="G77" s="35"/>
@@ -7579,10 +7594,10 @@
         <v>69</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E78" s="32" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F78" s="35"/>
       <c r="G78" s="35"/>
@@ -7616,10 +7631,10 @@
         <v>69</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F79" s="35"/>
       <c r="G79" s="35"/>
@@ -7653,10 +7668,10 @@
         <v>69</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F80" s="35"/>
       <c r="G80" s="35"/>
@@ -7690,10 +7705,10 @@
         <v>69</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F81" s="35"/>
       <c r="G81" s="35"/>
@@ -7727,10 +7742,10 @@
         <v>71</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E82" s="32" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F82" s="35"/>
       <c r="G82" s="35"/>
@@ -7764,10 +7779,10 @@
         <v>71</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E83" s="32" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F83" s="35"/>
       <c r="G83" s="35"/>
@@ -7801,10 +7816,10 @@
         <v>71</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E84" s="32" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F84" s="35"/>
       <c r="G84" s="35"/>
@@ -7838,10 +7853,10 @@
         <v>71</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E85" s="32" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F85" s="35"/>
       <c r="G85" s="35"/>
@@ -7875,10 +7890,10 @@
         <v>71</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E86" s="32" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F86" s="35"/>
       <c r="G86" s="35"/>
@@ -7912,10 +7927,10 @@
         <v>71</v>
       </c>
       <c r="D87" s="29" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E87" s="32" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F87" s="35"/>
       <c r="G87" s="35"/>
@@ -7949,10 +7964,10 @@
         <v>71</v>
       </c>
       <c r="D88" s="29" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F88" s="35"/>
       <c r="G88" s="35"/>
@@ -7986,10 +8001,10 @@
         <v>71</v>
       </c>
       <c r="D89" s="29" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E89" s="32" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F89" s="35"/>
       <c r="G89" s="35"/>
@@ -8023,10 +8038,10 @@
         <v>71</v>
       </c>
       <c r="D90" s="29" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F90" s="35"/>
       <c r="G90" s="35"/>
@@ -8060,10 +8075,10 @@
         <v>71</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="F91" s="35"/>
       <c r="G91" s="35"/>
@@ -8097,10 +8112,10 @@
         <v>71</v>
       </c>
       <c r="D92" s="29" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E92" s="32" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="F92" s="35"/>
       <c r="G92" s="35"/>
@@ -8134,10 +8149,10 @@
         <v>71</v>
       </c>
       <c r="D93" s="29" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F93" s="35"/>
       <c r="G93" s="35"/>
@@ -8171,10 +8186,10 @@
         <v>71</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F94" s="35"/>
       <c r="G94" s="35"/>
@@ -8208,10 +8223,10 @@
         <v>73</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="F95" s="35"/>
       <c r="G95" s="35"/>
@@ -8245,10 +8260,10 @@
         <v>73</v>
       </c>
       <c r="D96" s="29" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F96" s="35"/>
       <c r="G96" s="35"/>
@@ -8282,10 +8297,10 @@
         <v>73</v>
       </c>
       <c r="D97" s="29" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="E97" s="32" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F97" s="35"/>
       <c r="G97" s="35"/>
@@ -8319,10 +8334,10 @@
         <v>73</v>
       </c>
       <c r="D98" s="29" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E98" s="32" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F98" s="35"/>
       <c r="G98" s="35"/>
@@ -8356,10 +8371,10 @@
         <v>73</v>
       </c>
       <c r="D99" s="29" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E99" s="32" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F99" s="35"/>
       <c r="G99" s="35"/>
@@ -8393,10 +8408,10 @@
         <v>73</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E100" s="32" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F100" s="35"/>
       <c r="G100" s="35"/>
@@ -8430,10 +8445,10 @@
         <v>73</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="E101" s="32" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F101" s="35"/>
       <c r="G101" s="35"/>
@@ -8467,10 +8482,10 @@
         <v>73</v>
       </c>
       <c r="D102" s="29" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E102" s="32" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F102" s="35"/>
       <c r="G102" s="35"/>
@@ -8504,10 +8519,10 @@
         <v>73</v>
       </c>
       <c r="D103" s="29" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E103" s="32" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F103" s="35"/>
       <c r="G103" s="35"/>
@@ -8541,10 +8556,10 @@
         <v>73</v>
       </c>
       <c r="D104" s="29" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E104" s="32" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="F104" s="35"/>
       <c r="G104" s="35"/>
@@ -8578,10 +8593,10 @@
         <v>73</v>
       </c>
       <c r="D105" s="29" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E105" s="32" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="F105" s="35"/>
       <c r="G105" s="35"/>
@@ -8615,10 +8630,10 @@
         <v>73</v>
       </c>
       <c r="D106" s="29" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E106" s="32" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F106" s="35"/>
       <c r="G106" s="35"/>
@@ -8652,10 +8667,10 @@
         <v>73</v>
       </c>
       <c r="D107" s="29" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E107" s="32" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F107" s="35"/>
       <c r="G107" s="35"/>
@@ -8689,10 +8704,10 @@
         <v>73</v>
       </c>
       <c r="D108" s="29" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E108" s="32" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="F108" s="35"/>
       <c r="G108" s="35"/>
@@ -8726,10 +8741,10 @@
         <v>73</v>
       </c>
       <c r="D109" s="29" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E109" s="32" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F109" s="35"/>
       <c r="G109" s="35"/>
@@ -8763,10 +8778,10 @@
         <v>73</v>
       </c>
       <c r="D110" s="29" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E110" s="32" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F110" s="35"/>
       <c r="G110" s="35"/>
@@ -8800,10 +8815,10 @@
         <v>73</v>
       </c>
       <c r="D111" s="29" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E111" s="32" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="F111" s="35"/>
       <c r="G111" s="35"/>
@@ -8837,10 +8852,10 @@
         <v>73</v>
       </c>
       <c r="D112" s="29" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E112" s="32" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="F112" s="35"/>
       <c r="G112" s="35"/>
@@ -8874,10 +8889,10 @@
         <v>73</v>
       </c>
       <c r="D113" s="29" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E113" s="32" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="F113" s="35"/>
       <c r="G113" s="35"/>
@@ -8911,10 +8926,10 @@
         <v>73</v>
       </c>
       <c r="D114" s="29" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E114" s="32" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F114" s="35"/>
       <c r="G114" s="35"/>
@@ -8948,10 +8963,10 @@
         <v>73</v>
       </c>
       <c r="D115" s="29" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E115" s="32" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F115" s="35"/>
       <c r="G115" s="35"/>
@@ -8985,10 +9000,10 @@
         <v>73</v>
       </c>
       <c r="D116" s="29" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E116" s="32" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F116" s="35"/>
       <c r="G116" s="35"/>
@@ -9022,10 +9037,10 @@
         <v>73</v>
       </c>
       <c r="D117" s="29" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="E117" s="32" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F117" s="35"/>
       <c r="G117" s="35"/>
@@ -9059,10 +9074,10 @@
         <v>67</v>
       </c>
       <c r="D118" s="29" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E118" s="32" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F118" s="35"/>
       <c r="G118" s="35"/>
@@ -9096,10 +9111,10 @@
         <v>67</v>
       </c>
       <c r="D119" s="29" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E119" s="32" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="F119" s="35"/>
       <c r="G119" s="35"/>
@@ -9133,10 +9148,10 @@
         <v>67</v>
       </c>
       <c r="D120" s="29" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E120" s="32" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F120" s="35"/>
       <c r="G120" s="35"/>
@@ -9170,10 +9185,10 @@
         <v>67</v>
       </c>
       <c r="D121" s="29" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E121" s="32" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="F121" s="35"/>
       <c r="G121" s="35"/>
@@ -9207,10 +9222,10 @@
         <v>67</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E122" s="32" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F122" s="35"/>
       <c r="G122" s="35"/>
@@ -9244,10 +9259,10 @@
         <v>67</v>
       </c>
       <c r="D123" s="29" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E123" s="32" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F123" s="35"/>
       <c r="G123" s="35"/>
@@ -9281,10 +9296,10 @@
         <v>67</v>
       </c>
       <c r="D124" s="29" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E124" s="32" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F124" s="35"/>
       <c r="G124" s="35"/>
@@ -9318,10 +9333,10 @@
         <v>67</v>
       </c>
       <c r="D125" s="29" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E125" s="32" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="F125" s="35"/>
       <c r="G125" s="35"/>
@@ -9355,10 +9370,10 @@
         <v>67</v>
       </c>
       <c r="D126" s="29" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E126" s="32" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F126" s="35"/>
       <c r="G126" s="35"/>
@@ -9392,10 +9407,10 @@
         <v>67</v>
       </c>
       <c r="D127" s="29" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="E127" s="32" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="F127" s="35"/>
       <c r="G127" s="35"/>
@@ -9429,10 +9444,10 @@
         <v>67</v>
       </c>
       <c r="D128" s="29" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E128" s="32" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="F128" s="35"/>
       <c r="G128" s="35"/>
@@ -9466,10 +9481,10 @@
         <v>67</v>
       </c>
       <c r="D129" s="29" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F129" s="35"/>
       <c r="G129" s="35"/>
@@ -9503,10 +9518,10 @@
         <v>67</v>
       </c>
       <c r="D130" s="29" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E130" s="32" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F130" s="35"/>
       <c r="G130" s="35"/>
@@ -9540,10 +9555,10 @@
         <v>67</v>
       </c>
       <c r="D131" s="29" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E131" s="32" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F131" s="35"/>
       <c r="G131" s="35"/>
@@ -9577,10 +9592,10 @@
         <v>67</v>
       </c>
       <c r="D132" s="29" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="E132" s="32" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="F132" s="35"/>
       <c r="G132" s="35"/>
@@ -9614,10 +9629,10 @@
         <v>67</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F133" s="35"/>
       <c r="G133" s="35"/>
@@ -9651,10 +9666,10 @@
         <v>63</v>
       </c>
       <c r="D134" s="29" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F134" s="35"/>
       <c r="G134" s="35"/>
@@ -9688,10 +9703,10 @@
         <v>63</v>
       </c>
       <c r="D135" s="29" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F135" s="35"/>
       <c r="G135" s="35"/>
@@ -9725,10 +9740,10 @@
         <v>63</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E136" s="32" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="F136" s="35"/>
       <c r="G136" s="35"/>
@@ -9762,10 +9777,10 @@
         <v>63</v>
       </c>
       <c r="D137" s="29" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="E137" s="32" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F137" s="35"/>
       <c r="G137" s="35"/>
@@ -9799,10 +9814,10 @@
         <v>63</v>
       </c>
       <c r="D138" s="29" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="E138" s="32" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F138" s="35"/>
       <c r="G138" s="35"/>
@@ -9836,10 +9851,10 @@
         <v>63</v>
       </c>
       <c r="D139" s="29" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E139" s="32" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F139" s="35"/>
       <c r="G139" s="35"/>
@@ -9873,10 +9888,10 @@
         <v>63</v>
       </c>
       <c r="D140" s="29" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="E140" s="32" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F140" s="35"/>
       <c r="G140" s="35"/>
@@ -9910,10 +9925,10 @@
         <v>63</v>
       </c>
       <c r="D141" s="29" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="E141" s="32" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="F141" s="35"/>
       <c r="G141" s="35"/>
@@ -9947,10 +9962,10 @@
         <v>63</v>
       </c>
       <c r="D142" s="29" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E142" s="32" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F142" s="35"/>
       <c r="G142" s="35"/>
@@ -9984,10 +9999,10 @@
         <v>63</v>
       </c>
       <c r="D143" s="29" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="E143" s="32" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="F143" s="35"/>
       <c r="G143" s="35"/>
@@ -10021,10 +10036,10 @@
         <v>63</v>
       </c>
       <c r="D144" s="29" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="E144" s="32" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F144" s="35"/>
       <c r="G144" s="35"/>
@@ -10058,10 +10073,10 @@
         <v>63</v>
       </c>
       <c r="D145" s="29" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="E145" s="32" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="F145" s="35"/>
       <c r="G145" s="35"/>
@@ -10095,10 +10110,10 @@
         <v>63</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="E146" s="32" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="F146" s="35"/>
       <c r="G146" s="35"/>
@@ -10132,10 +10147,10 @@
         <v>63</v>
       </c>
       <c r="D147" s="29" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="E147" s="32" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F147" s="35"/>
       <c r="G147" s="35"/>
@@ -10169,10 +10184,10 @@
         <v>63</v>
       </c>
       <c r="D148" s="29" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="E148" s="32" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="F148" s="35"/>
       <c r="G148" s="35"/>
@@ -10206,10 +10221,10 @@
         <v>48</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="E149" s="32" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="F149" s="35"/>
       <c r="G149" s="35"/>
@@ -10219,7 +10234,7 @@
         <v>58</v>
       </c>
       <c r="K149" s="37" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="L149" s="37"/>
       <c r="M149" s="37"/>
@@ -10247,10 +10262,10 @@
         <v>48</v>
       </c>
       <c r="D150" s="29" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="E150" s="32" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="F150" s="35"/>
       <c r="G150" s="35"/>
@@ -10260,7 +10275,7 @@
         <v>58</v>
       </c>
       <c r="K150" s="37" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="L150" s="37"/>
       <c r="M150" s="37"/>
@@ -10285,13 +10300,13 @@
         <v>47</v>
       </c>
       <c r="C151" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D151" s="29" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="E151" s="32" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F151" s="35"/>
       <c r="G151" s="35"/>
@@ -10322,13 +10337,13 @@
         <v>47</v>
       </c>
       <c r="C152" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D152" s="29" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="E152" s="32" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="F152" s="35"/>
       <c r="G152" s="35"/>
@@ -10359,13 +10374,13 @@
         <v>47</v>
       </c>
       <c r="C153" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D153" s="29" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="E153" s="32" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="F153" s="35"/>
       <c r="G153" s="35"/>
@@ -10396,10 +10411,10 @@
         <v>47</v>
       </c>
       <c r="C154" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D154" s="29" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E154" s="32" t="s">
         <v>57</v>
@@ -10433,10 +10448,10 @@
         <v>47</v>
       </c>
       <c r="C155" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D155" s="29" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="E155" s="32" t="s">
         <v>76</v>
@@ -10470,13 +10485,13 @@
         <v>47</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D156" s="29" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="E156" s="32" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="F156" s="35"/>
       <c r="G156" s="35"/>
@@ -10507,13 +10522,13 @@
         <v>47</v>
       </c>
       <c r="C157" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D157" s="29" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="E157" s="32" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="F157" s="35"/>
       <c r="G157" s="35"/>
@@ -10544,13 +10559,13 @@
         <v>47</v>
       </c>
       <c r="C158" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D158" s="29" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E158" s="32" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="F158" s="35"/>
       <c r="G158" s="35"/>
@@ -10581,13 +10596,13 @@
         <v>47</v>
       </c>
       <c r="C159" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D159" s="29" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="E159" s="32" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="F159" s="35"/>
       <c r="G159" s="35"/>
@@ -10618,13 +10633,13 @@
         <v>47</v>
       </c>
       <c r="C160" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D160" s="29" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="E160" s="32" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="F160" s="35"/>
       <c r="G160" s="35"/>
@@ -10655,13 +10670,13 @@
         <v>47</v>
       </c>
       <c r="C161" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D161" s="29" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="E161" s="32" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="F161" s="35"/>
       <c r="G161" s="35"/>
@@ -10692,13 +10707,13 @@
         <v>47</v>
       </c>
       <c r="C162" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D162" s="29" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="E162" s="32" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="F162" s="35"/>
       <c r="G162" s="35"/>
@@ -10729,13 +10744,13 @@
         <v>47</v>
       </c>
       <c r="C163" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D163" s="29" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="E163" s="32" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="F163" s="35"/>
       <c r="G163" s="35"/>
@@ -10766,13 +10781,13 @@
         <v>47</v>
       </c>
       <c r="C164" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D164" s="29" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="E164" s="32" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="F164" s="35"/>
       <c r="G164" s="35"/>
@@ -10803,13 +10818,13 @@
         <v>47</v>
       </c>
       <c r="C165" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D165" s="29" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="E165" s="32" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="F165" s="35"/>
       <c r="G165" s="35"/>
@@ -10840,13 +10855,13 @@
         <v>47</v>
       </c>
       <c r="C166" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D166" s="29" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="E166" s="32" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="F166" s="35"/>
       <c r="G166" s="35"/>
@@ -10880,10 +10895,10 @@
         <v>63</v>
       </c>
       <c r="D167" s="29" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="E167" s="32" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="F167" s="35"/>
       <c r="G167" s="35"/>
@@ -10917,10 +10932,10 @@
         <v>63</v>
       </c>
       <c r="D168" s="29" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E168" s="32" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="F168" s="35"/>
       <c r="G168" s="35"/>
@@ -10954,10 +10969,10 @@
         <v>67</v>
       </c>
       <c r="D169" s="29" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="E169" s="32" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="F169" s="35"/>
       <c r="G169" s="35"/>
@@ -10991,10 +11006,10 @@
         <v>67</v>
       </c>
       <c r="D170" s="29" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="E170" s="32" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="F170" s="35"/>
       <c r="G170" s="35"/>
@@ -11028,10 +11043,10 @@
         <v>61</v>
       </c>
       <c r="D171" s="29" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="E171" s="32" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="F171" s="35"/>
       <c r="G171" s="35"/>
@@ -11065,10 +11080,10 @@
         <v>61</v>
       </c>
       <c r="D172" s="29" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="E172" s="32" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="F172" s="35"/>
       <c r="G172" s="35"/>
@@ -11102,22 +11117,22 @@
         <v>48</v>
       </c>
       <c r="D173" s="29" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="E173" s="32" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="F173" s="35">
         <v>45798</v>
       </c>
       <c r="G173" s="35" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="H173" s="35" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="I173" s="38" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="J173" s="37" t="s">
         <v>54</v>
@@ -11149,10 +11164,10 @@
         <v>73</v>
       </c>
       <c r="D174" s="29" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E174" s="32" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="F174" s="35"/>
       <c r="G174" s="35"/>
@@ -11186,10 +11201,10 @@
         <v>73</v>
       </c>
       <c r="D175" s="29" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E175" s="32" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="F175" s="35"/>
       <c r="G175" s="35"/>
@@ -11223,10 +11238,10 @@
         <v>71</v>
       </c>
       <c r="D176" s="29" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="E176" s="32" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="F176" s="35"/>
       <c r="G176" s="35"/>
@@ -11260,10 +11275,10 @@
         <v>71</v>
       </c>
       <c r="D177" s="29" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="E177" s="32" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="F177" s="35"/>
       <c r="G177" s="35"/>
@@ -11297,10 +11312,10 @@
         <v>69</v>
       </c>
       <c r="D178" s="29" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="E178" s="32" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="F178" s="35"/>
       <c r="G178" s="35"/>
@@ -11334,10 +11349,10 @@
         <v>69</v>
       </c>
       <c r="D179" s="29" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E179" s="32" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="F179" s="35"/>
       <c r="G179" s="35"/>
@@ -11368,13 +11383,13 @@
         <v>47</v>
       </c>
       <c r="C180" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D180" s="29" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="E180" s="32" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="F180" s="35"/>
       <c r="G180" s="35"/>
@@ -11408,10 +11423,10 @@
         <v>67</v>
       </c>
       <c r="D181" s="29" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E181" s="32" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="F181" s="29"/>
       <c r="G181" s="29"/>
@@ -11445,10 +11460,10 @@
         <v>65</v>
       </c>
       <c r="D182" s="29" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="E182" s="32" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="F182" s="29"/>
       <c r="G182" s="29"/>
@@ -11482,10 +11497,10 @@
         <v>73</v>
       </c>
       <c r="D183" s="29" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="E183" s="32" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="F183" s="29"/>
       <c r="G183" s="29"/>
@@ -11519,10 +11534,10 @@
         <v>69</v>
       </c>
       <c r="D184" s="29" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="E184" s="32" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="F184" s="29"/>
       <c r="G184" s="29"/>
@@ -11556,10 +11571,10 @@
         <v>71</v>
       </c>
       <c r="D185" s="29" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="E185" s="32" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="F185" s="29"/>
       <c r="G185" s="29"/>
@@ -11593,10 +11608,10 @@
         <v>48</v>
       </c>
       <c r="D186" s="29" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="E186" s="32" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="F186" s="29"/>
       <c r="G186" s="29"/>
@@ -11606,7 +11621,7 @@
         <v>58</v>
       </c>
       <c r="K186" s="37" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="L186" s="29"/>
       <c r="M186" s="37"/>
@@ -11634,10 +11649,10 @@
         <v>61</v>
       </c>
       <c r="D187" s="29" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E187" s="32" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="F187" s="29"/>
       <c r="G187" s="29"/>
@@ -11671,10 +11686,10 @@
         <v>67</v>
       </c>
       <c r="D188" s="29" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="E188" s="32" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="F188" s="29"/>
       <c r="G188" s="29"/>
@@ -11708,10 +11723,10 @@
         <v>63</v>
       </c>
       <c r="D189" s="29" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="E189" s="32" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="F189" s="29"/>
       <c r="G189" s="29"/>
@@ -11742,13 +11757,13 @@
         <v>47</v>
       </c>
       <c r="C190" s="30" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D190" s="29" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E190" s="32" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F190" s="29"/>
       <c r="G190" s="29"/>
@@ -11782,10 +11797,10 @@
         <v>65</v>
       </c>
       <c r="D191" s="29" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E191" s="32" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F191" s="35"/>
       <c r="G191" s="35"/>
@@ -11819,10 +11834,10 @@
         <v>65</v>
       </c>
       <c r="D192" s="29" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="E192" s="32" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="F192" s="35"/>
       <c r="G192" s="35"/>
@@ -15970,32 +15985,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -16005,7 +16020,7 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -16038,22 +16053,22 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:4">
@@ -16061,13 +16076,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:4">
@@ -16075,13 +16090,13 @@
         <v>61</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:4">
@@ -16089,13 +16104,13 @@
         <v>65</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:4">
@@ -16103,13 +16118,13 @@
         <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:4">
@@ -16117,13 +16132,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -16131,13 +16146,13 @@
         <v>73</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -16145,13 +16160,13 @@
         <v>67</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -16159,41 +16174,41 @@
         <v>63</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="10" ht="30" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="4:4">
@@ -17185,7 +17200,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>54</v>
@@ -17193,7 +17208,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Aggiornamento dati versione 2.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.0/report-checklist.xlsx
@@ -278,13 +278,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-22T13:48:23Z</t>
-  </si>
-  <si>
-    <t>e9f7d206a5ae691b5c2fe0bc0b92a83c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.a5d629f814^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:46:58Z</t>
+  </si>
+  <si>
+    <t>119f46b6a9c297f0fa772efc0c3067d1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b3a5ec1907^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -504,13 +504,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-12T14:25:20Z</t>
-  </si>
-  <si>
-    <t>2abff759721e14cf4e6afd9cc3dc118b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.3606261b18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:01Z</t>
+  </si>
+  <si>
+    <t>34b8c9445a1809c2cd147c9693f08745</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.4f0db80cc4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE ERRORE FORMALE CODICE FISCALE</t>
@@ -526,13 +526,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:06:24Z</t>
-  </si>
-  <si>
-    <t>ce2dbf04bf119209c0b89d9ccd9ec523</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.e2b26f8051^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:04Z</t>
+  </si>
+  <si>
+    <t>1c0f7d4015117c3ea54e34a5a012bf70</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.643a20dde8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA IL COMUNE DI RESIDENZA</t>
@@ -548,13 +548,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:08:02Z</t>
-  </si>
-  <si>
-    <t>24943690b6d99363d7e3193728e8a1df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.cba3a4bc8f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:07Z</t>
+  </si>
+  <si>
+    <t>ee63eb1efc8a56eb3f8092666e33c68a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.516cd15872^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA IL NOME DEL PAZIENTE</t>
@@ -567,13 +567,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:09:16Z</t>
-  </si>
-  <si>
-    <t>ea789b4583569c72c376460af9afe2d3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.3dbdfcd50a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:10Z</t>
+  </si>
+  <si>
+    <t>3c16fd0823dfdb7f221171c5f45bd6a6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.5979ecdee6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA IL SESSO DEL PAZIENTE</t>
@@ -586,13 +586,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:11:24Z</t>
-  </si>
-  <si>
-    <t>7c8ae8ab860b98e1f4eced9461d09c9e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.4043cf18cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:13Z</t>
+  </si>
+  <si>
+    <t>55eb32148fe033dc94432f3558bca66a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.ed226c0528^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE ERRORE SULL'IDENTIFICATIVO UNIVOCO DELLA PRESCRIZIONE</t>
@@ -608,13 +608,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:12:21Z</t>
-  </si>
-  <si>
-    <t>65b7f36a06fe71bca965d340b8157beb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b40e844989^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:17Z</t>
+  </si>
+  <si>
+    <t>bf7e466638db03ac83b2fd192341c382</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.45fb880736^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE SPECIFICA ESAME NON CORRETTA</t>
@@ -630,13 +630,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:13:18Z</t>
-  </si>
-  <si>
-    <t>7fbf9aa54e7714342294e1aa644ebb0f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.f68c9c6a69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:20Z</t>
+  </si>
+  <si>
+    <t>aeea2044ad677b0ab228e75039a5d37f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.927bb74b39^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA LA SPECIFICA DEL TIPO DI CAMPIONE</t>
@@ -649,13 +649,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:14:13Z</t>
-  </si>
-  <si>
-    <t>ed85c21baa7c707660546343eb9f3cd5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.683ad8df8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:24Z</t>
+  </si>
+  <si>
+    <t>075c50d9e8a564d625e283bad5431775</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.ad1ad0040a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA LA SPECIFICA DEL CODICE DELL'ESAME ISOLATO</t>
@@ -1562,13 +1562,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-21T17:23:16Z</t>
-  </si>
-  <si>
-    <t>b0b335b83a2bd62cf5740145123d9525</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.12dbe02e35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:27Z</t>
+  </si>
+  <si>
+    <t>2ac8de5805465911f4a2fdf07d59dd05</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.19e7c3abc5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT30</t>
@@ -1711,13 +1711,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-06-06T11:00:21Z</t>
-  </si>
-  <si>
-    <t>2727cc18a4583582b4f33d16ca7133f1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.aa8bec23d0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T15:47:30Z</t>
+  </si>
+  <si>
+    <t>302e99ff2d2f0d8a7273789417a3197f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.c400963de2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE CODICE DI PRIORITA' DELLA RICHIESTA ERRATO</t>
@@ -1850,11 +1850,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1949,22 +1949,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1972,9 +1956,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2004,30 +1988,16 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2049,13 +2019,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2063,16 +2026,53 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2133,7 +2133,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2145,19 +2241,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2169,145 +2307,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2650,15 +2650,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -2679,17 +2670,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2701,15 +2681,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2728,143 +2699,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="30" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4511,11 +4511,11 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:D5"/>
+      <selection pane="bottomRight" activeCell="I190" sqref="I190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4533333333333" defaultRowHeight="15" customHeight="1"/>
@@ -4816,7 +4816,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="33">
-        <v>45799</v>
+        <v>45825</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>50</v>
@@ -5463,7 +5463,7 @@
         <v>84</v>
       </c>
       <c r="F27" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
@@ -5793,7 +5793,7 @@
         <v>95</v>
       </c>
       <c r="F35" s="34">
-        <v>45789</v>
+        <v>45825</v>
       </c>
       <c r="G35" s="34" t="s">
         <v>96</v>
@@ -5854,7 +5854,7 @@
         <v>102</v>
       </c>
       <c r="F36" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G36" s="34" t="s">
         <v>103</v>
@@ -5915,7 +5915,7 @@
         <v>109</v>
       </c>
       <c r="F37" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G37" s="34" t="s">
         <v>110</v>
@@ -5976,7 +5976,7 @@
         <v>115</v>
       </c>
       <c r="F38" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G38" s="34" t="s">
         <v>116</v>
@@ -6037,7 +6037,7 @@
         <v>121</v>
       </c>
       <c r="F39" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G39" s="34" t="s">
         <v>122</v>
@@ -6098,7 +6098,7 @@
         <v>128</v>
       </c>
       <c r="F40" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G40" s="34" t="s">
         <v>129</v>
@@ -6159,7 +6159,7 @@
         <v>135</v>
       </c>
       <c r="F41" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G41" s="34" t="s">
         <v>136</v>
@@ -6220,7 +6220,7 @@
         <v>141</v>
       </c>
       <c r="F42" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G42" s="34" t="s">
         <v>142</v>
@@ -10988,7 +10988,7 @@
         <v>401</v>
       </c>
       <c r="F170" s="34">
-        <v>45798</v>
+        <v>45825</v>
       </c>
       <c r="G170" s="34" t="s">
         <v>402</v>
@@ -11742,7 +11742,7 @@
         <v>444</v>
       </c>
       <c r="F190" s="34">
-        <v>45814</v>
+        <v>45825</v>
       </c>
       <c r="G190" s="34" t="s">
         <v>445</v>

</xml_diff>

<commit_message>
Reinvio dati di tracciabilita`  versione 2.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.0/report-checklist.xlsx
@@ -278,13 +278,13 @@
 </t>
   </si>
   <si>
-    <t>2025-06-17T15:46:58Z</t>
-  </si>
-  <si>
-    <t>119f46b6a9c297f0fa772efc0c3067d1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b3a5ec1907^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-20T06:40:27Z</t>
+  </si>
+  <si>
+    <t>2736bbbfc98d14cf575039311a5080e0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.e66efe93c2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -1562,13 +1562,13 @@
 </t>
   </si>
   <si>
-    <t>2025-06-17T15:47:27Z</t>
-  </si>
-  <si>
-    <t>2ac8de5805465911f4a2fdf07d59dd05</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.19e7c3abc5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-20T06:45:32Z</t>
+  </si>
+  <si>
+    <t>569afaa0245329ee168c14e993110dfe</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b817513fc0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT30</t>
@@ -1851,10 +1851,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1956,14 +1956,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1971,11 +1963,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1989,7 +1997,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2003,16 +2026,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2033,14 +2048,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -2048,23 +2055,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2072,7 +2064,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2133,7 +2133,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2145,13 +2163,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2163,19 +2181,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2187,7 +2235,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2199,55 +2277,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2259,55 +2307,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2631,6 +2631,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2642,15 +2666,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2670,17 +2685,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2702,17 +2713,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -2724,7 +2724,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2735,136 +2735,136 @@
     <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4511,11 +4511,11 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E170" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I190" sqref="I190"/>
+      <selection pane="bottomRight" activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4533333333333" defaultRowHeight="15" customHeight="1"/>
@@ -4816,7 +4816,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="33">
-        <v>45825</v>
+        <v>45828</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>50</v>
@@ -10988,7 +10988,7 @@
         <v>401</v>
       </c>
       <c r="F170" s="34">
-        <v>45825</v>
+        <v>45828</v>
       </c>
       <c r="G170" s="34" t="s">
         <v>402</v>

</xml_diff>